<commit_message>
coding for rest of PfG covariates added - RF
</commit_message>
<xml_diff>
--- a/code/pfg_tables/Classifications_Equality Groups - Template.xlsx
+++ b/code/pfg_tables/Classifications_Equality Groups - Template.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2337714\Documents\R\71-ssb-pcos\code\pfg tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1251607\Documents\R\pcos-2024\code\pfg_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75379F7-0E9A-44C3-AEA9-6D5F440E2D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E97B5B-CE30-4B7B-B75C-87564AFEAEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="615" windowWidth="28500" windowHeight="20985" activeTab="1" xr2:uid="{90E7B0A8-FD23-4CBE-8759-8E7916B7D001}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{90E7B0A8-FD23-4CBE-8759-8E7916B7D001}"/>
   </bookViews>
   <sheets>
     <sheet name="Advice" sheetId="2" r:id="rId1"/>
     <sheet name="Classifications_EQ - Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Classifications_LGD - Template" sheetId="4" r:id="rId3"/>
+    <sheet name="Classifications_AA - Template" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Classifications_AA - Template'!$A$2:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classifications_EQ - Template'!$A$2:$C$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Classifications_LGD - Template'!$A$2:$C$13</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
   <si>
     <t>CODE</t>
   </si>
@@ -300,6 +304,180 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Local Government District</t>
+  </si>
+  <si>
+    <t>Antrim and Newtownabbey</t>
+  </si>
+  <si>
+    <t>Armagh, Banbridge and Craigavon</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Causeway Coast and Glens</t>
+  </si>
+  <si>
+    <t>Derry and Strabane</t>
+  </si>
+  <si>
+    <t>Fermanagh and Omagh</t>
+  </si>
+  <si>
+    <t>Lisburn and Castlereagh</t>
+  </si>
+  <si>
+    <t>Mid and East Antrim</t>
+  </si>
+  <si>
+    <t>Newry, Mourne and Down</t>
+  </si>
+  <si>
+    <t>North Down and Ards</t>
+  </si>
+  <si>
+    <t>Belfast East</t>
+  </si>
+  <si>
+    <t>Belfast North</t>
+  </si>
+  <si>
+    <t>Belfast South</t>
+  </si>
+  <si>
+    <t>Belfast West</t>
+  </si>
+  <si>
+    <t>East Antrim</t>
+  </si>
+  <si>
+    <t>East Londonderry</t>
+  </si>
+  <si>
+    <t>Fermanagh and South Tyrone</t>
+  </si>
+  <si>
+    <t>Foyle</t>
+  </si>
+  <si>
+    <t>Lagan Valley</t>
+  </si>
+  <si>
+    <t>Mid Ulster</t>
+  </si>
+  <si>
+    <t>Newry and Armagh</t>
+  </si>
+  <si>
+    <t>North Antrim</t>
+  </si>
+  <si>
+    <t>North Down</t>
+  </si>
+  <si>
+    <t>South Antrim</t>
+  </si>
+  <si>
+    <t>South Down</t>
+  </si>
+  <si>
+    <t>Strangford</t>
+  </si>
+  <si>
+    <t>Upper Bann</t>
+  </si>
+  <si>
+    <t>West Tyrone</t>
+  </si>
+  <si>
+    <t>Assembly Area</t>
+  </si>
+  <si>
+    <t>N09000001</t>
+  </si>
+  <si>
+    <t>N09000002</t>
+  </si>
+  <si>
+    <t>N09000003</t>
+  </si>
+  <si>
+    <t>N09000004</t>
+  </si>
+  <si>
+    <t>N09000005</t>
+  </si>
+  <si>
+    <t>N09000006</t>
+  </si>
+  <si>
+    <t>N09000007</t>
+  </si>
+  <si>
+    <t>N09000008</t>
+  </si>
+  <si>
+    <t>N09000009</t>
+  </si>
+  <si>
+    <t>N09000010</t>
+  </si>
+  <si>
+    <t>N09000011</t>
+  </si>
+  <si>
+    <t>N06000001</t>
+  </si>
+  <si>
+    <t>N06000002</t>
+  </si>
+  <si>
+    <t>N06000003</t>
+  </si>
+  <si>
+    <t>N06000004</t>
+  </si>
+  <si>
+    <t>N06000005</t>
+  </si>
+  <si>
+    <t>N06000006</t>
+  </si>
+  <si>
+    <t>N06000007</t>
+  </si>
+  <si>
+    <t>N06000008</t>
+  </si>
+  <si>
+    <t>N06000009</t>
+  </si>
+  <si>
+    <t>N06000010</t>
+  </si>
+  <si>
+    <t>N06000011</t>
+  </si>
+  <si>
+    <t>N06000012</t>
+  </si>
+  <si>
+    <t>N06000013</t>
+  </si>
+  <si>
+    <t>N06000014</t>
+  </si>
+  <si>
+    <t>N06000015</t>
+  </si>
+  <si>
+    <t>N06000016</t>
+  </si>
+  <si>
+    <t>N06000017</t>
   </si>
 </sst>
 </file>
@@ -1224,14 +1402,14 @@
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1246,18 +1424,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AB9F98-9008-42A6-9974-F0B1D0C756EC}">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1276,7 +1454,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1288,7 +1466,7 @@
         <v xml:space="preserve">Sex </v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1300,7 +1478,7 @@
         <v xml:space="preserve">Sex </v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1312,7 +1490,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1324,7 +1502,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1336,7 +1514,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1348,7 +1526,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1360,7 +1538,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1372,7 +1550,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1384,7 +1562,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1396,7 +1574,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1408,7 +1586,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1420,7 +1598,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1432,7 +1610,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1444,7 +1622,7 @@
         <v xml:space="preserve">Religion </v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1456,7 +1634,7 @@
         <v xml:space="preserve">Religion </v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1468,7 +1646,7 @@
         <v xml:space="preserve">Religion </v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1480,7 +1658,7 @@
         <v xml:space="preserve">Dependants </v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1492,7 +1670,7 @@
         <v xml:space="preserve">Dependants </v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1504,7 +1682,7 @@
         <v xml:space="preserve">Disability </v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1516,7 +1694,7 @@
         <v xml:space="preserve">Disability </v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1528,7 +1706,7 @@
         <v xml:space="preserve">Ethnic group </v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1540,7 +1718,7 @@
         <v xml:space="preserve">Ethnic group </v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1552,7 +1730,7 @@
         <v>Sexual orientation</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1564,7 +1742,7 @@
         <v xml:space="preserve">Sexual orientation </v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1576,7 +1754,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1588,7 +1766,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1600,7 +1778,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1612,7 +1790,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1624,7 +1802,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1636,7 +1814,7 @@
         <v xml:space="preserve">Urban Rural </v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1648,7 +1826,7 @@
         <v xml:space="preserve">Urban Rural </v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1660,7 +1838,7 @@
         <v xml:space="preserve">Urban Rural </v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1672,7 +1850,7 @@
         <v xml:space="preserve">Political opinion </v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1684,7 +1862,7 @@
         <v xml:space="preserve">Political opinion </v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1696,7 +1874,7 @@
         <v xml:space="preserve">Political opinion </v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1708,7 +1886,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1720,7 +1898,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1732,7 +1910,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1744,7 +1922,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1756,7 +1934,7 @@
         <v xml:space="preserve">Deprivation </v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1768,7 +1946,7 @@
         <v xml:space="preserve">Marital status </v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1780,7 +1958,7 @@
         <v xml:space="preserve">Tenure </v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1792,7 +1970,7 @@
         <v xml:space="preserve">Tenure </v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1804,7 +1982,7 @@
         <v xml:space="preserve">Tenure </v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1816,7 +1994,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1828,7 +2006,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1840,7 +2018,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1852,7 +2030,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1864,7 +2042,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1876,7 +2054,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1888,7 +2066,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1900,7 +2078,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1912,7 +2090,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1924,7 +2102,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1936,7 +2114,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1948,7 +2126,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1960,7 +2138,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1972,7 +2150,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1984,7 +2162,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1996,7 +2174,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2008,7 +2186,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2020,7 +2198,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2032,7 +2210,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2044,7 +2222,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2056,7 +2234,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2068,7 +2246,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2080,7 +2258,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2092,7 +2270,7 @@
         <v xml:space="preserve">Household Group </v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2104,7 +2282,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2116,7 +2294,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2128,7 +2306,7 @@
         <v>Age</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
     </row>
   </sheetData>
@@ -2136,4 +2314,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3010A9-2D03-4B29-9345-2C9FE5DEA016}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:C13" xr:uid="{98AB9F98-9008-42A6-9974-F0B1D0C756EC}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C227AAC-1AEF-48F5-84A8-0EA2349BE270}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:C20" xr:uid="{98AB9F98-9008-42A6-9974-F0B1D0C756EC}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>